<commit_message>
Move some small traces a little, update BOMs
</commit_message>
<xml_diff>
--- a/hardware/DC27-Cylon-BOM.xlsx
+++ b/hardware/DC27-Cylon-BOM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t xml:space="preserve">Battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAO</t>
   </si>
 </sst>
 </file>
@@ -169,6 +175,7 @@
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,6 +191,65 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -191,76 +257,29 @@
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -272,8 +291,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -284,32 +327,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -361,23 +380,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -392,23 +445,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -478,10 +531,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -489,7 +542,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.08"/>
   </cols>
   <sheetData>
@@ -711,6 +764,23 @@
         <v>37</v>
       </c>
       <c r="E13" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>